<commit_message>
Added new sequence diagrams
</commit_message>
<xml_diff>
--- a/Use Case Descriptions.xlsx
+++ b/Use Case Descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niel/Documents/!TPADesktop/TPA-Desktop-LinKasa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251C09F6-F9DE-1145-9847-E5D582545D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5261D73-35D8-E543-9278-1F996363EF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3500" yWindow="740" windowWidth="24720" windowHeight="16720" activeTab="1" xr2:uid="{B1ED97EC-A297-DE45-89E2-47350D4B0270}"/>
   </bookViews>
@@ -1218,17 +1218,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1365,17 +1365,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1512,17 +1512,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1659,17 +1659,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1806,17 +1806,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1953,17 +1953,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Use Case Description
</commit_message>
<xml_diff>
--- a/Use Case Descriptions.xlsx
+++ b/Use Case Descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niel/Documents/!TPADesktop/TPA-Desktop-LinKasa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5261D73-35D8-E543-9278-1F996363EF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E89130-EC08-4B41-A81D-DB9D425B873C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="740" windowWidth="24720" windowHeight="16720" activeTab="1" xr2:uid="{B1ED97EC-A297-DE45-89E2-47350D4B0270}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24720" windowHeight="16720" activeTab="5" xr2:uid="{B1ED97EC-A297-DE45-89E2-47350D4B0270}"/>
   </bookViews>
   <sheets>
     <sheet name="Update Lost and Found Entry" sheetId="1" r:id="rId1"/>
@@ -95,15 +95,6 @@
     <t>Lost and Found Staff</t>
   </si>
   <si>
-    <t>Staffs have to view the lost and found log in order to update it.</t>
-  </si>
-  <si>
-    <t>Everyone at the airport who lost or find an item.</t>
-  </si>
-  <si>
-    <t>2.1 One of the data isn't filled.</t>
-  </si>
-  <si>
     <t>The digital log is successfully updated along with the items information.
 The status of the lost item is updated based on staff's action.
 The updated information is stored inside the database.</t>
@@ -168,9 +159,6 @@
     <t>Provide Baggage Information</t>
   </si>
   <si>
-    <t>Provide detailed baggage information such as weight, dimensions, content, etc.</t>
-  </si>
-  <si>
     <t>Flight operations manager create a new flight schedule to fulfill passenger's high demand on tickets.</t>
   </si>
   <si>
@@ -226,9 +214,6 @@
     <t>Flight Operations Manager</t>
   </si>
   <si>
-    <t>Flight Operations Manager have to open the Flight Crew List Page before assigning any flight crews.</t>
-  </si>
-  <si>
     <t>Flight Attendants, Pilot</t>
   </si>
   <si>
@@ -264,15 +249,6 @@
     <t>Input Passenger Personal Information, Passport, and Visa Details</t>
   </si>
   <si>
-    <t>Customs and Border Control Officer could manually input the passenger's personal information before entering the departures waiting room.</t>
-  </si>
-  <si>
-    <t>Data in the "Access Passenger Information" use case will be updated after the following use case successfully executed.</t>
-  </si>
-  <si>
-    <t>Passengers traveling international within the airport.</t>
-  </si>
-  <si>
     <t>Passenger information will be stored into database.
 Newly stored data will be updated along the system.</t>
   </si>
@@ -304,9 +280,6 @@
     <t>Human Resources Director</t>
   </si>
   <si>
-    <t>Human Resources Director could insert new staff data into database for recently hired staff based on their data.</t>
-  </si>
-  <si>
     <t>The data in "View detailed employee data" use case will be updated after executing the following use case.</t>
   </si>
   <si>
@@ -378,11 +351,6 @@
 Baggage information such as dimensions, weight, and contents must be provided.</t>
   </si>
   <si>
-    <t>Lost and found staff must be logged in and authorized to update lost and found entry.
-The digital log must be created.
-A lost item has been reported.</t>
-  </si>
-  <si>
     <t>1.1 System opens chat room.
 1.2 System prompts actor to input public chat.
 2.1 System uploads sent chat to database.
@@ -404,6 +372,39 @@
     <t>Actor must be logged in and authorized to create flight schedule.
 Real-time flight schedule must exist.
 New flight schedule created must be unique.</t>
+  </si>
+  <si>
+    <t>View lost and found entry</t>
+  </si>
+  <si>
+    <t>Customer Service Manager, Information Desk Staff, Lost and Found Staff, Check-in Staff, Gate Agents, Airport Operations Manager, Flight Operations Manager, Ground Handling Manager, Landside Operations Manager, Maintenance Manager, Customs and Border Control Officers, Baggage Security Supervisor, Cargo Manager, Logistics Manager, Fuel Manager, Cargo Handlers, Civil Engineering Manager, Airport Director/CEO, Chief Financial Officer, Chief Operations Officer, Chief Security Officer, Human Resources Director</t>
+  </si>
+  <si>
+    <t>Lost and found staff must be logged in and authorized to update lost and found entry.
+Lost and found log must exists.
+The digital log must be created.
+A lost item has been reported.</t>
+  </si>
+  <si>
+    <t>2.1 Some of the data is incomplete or status is not selected</t>
+  </si>
+  <si>
+    <t>Provide detailed baggage information such as weight, dimensions, content, and attach photos.</t>
+  </si>
+  <si>
+    <t>View flight crews, Access passenger information</t>
+  </si>
+  <si>
+    <t>Access Passenger Information</t>
+  </si>
+  <si>
+    <t>Passenger, Check-in Staff, Customs and Border Control Officers, Flight Operations Manager, Gate Agents</t>
+  </si>
+  <si>
+    <t>Customs and Border Control Officer could manually input the passenger's personal information such as Full Name, Date of Birth, Nationality, Passport Number, and Visa details before entering the departures waiting room.</t>
+  </si>
+  <si>
+    <t>Human Resources Director could insert new staff data such as name, role, address, date of birth into database, then generate email and password for recently hired staff.</t>
   </si>
 </sst>
 </file>
@@ -592,9 +593,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -610,9 +608,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -627,6 +622,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABC9673-1384-A541-9754-03D8B487CAC3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView topLeftCell="A8" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -960,82 +961,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="19"/>
+      <c r="B3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1051,20 +1052,20 @@
     <row r="11" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="11"/>
+      <c r="B12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1091,7 +1092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F06FCE-2A99-3641-B0B3-A6FEC9347627}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="112" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
@@ -1107,82 +1108,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="13"/>
+      <c r="B2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="15"/>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1198,37 +1199,37 @@
     <row r="11" spans="1:3" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="21"/>
+      <c r="B12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1238,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D95F47F-4C81-BA4D-8C18-41A8801B31B5}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1254,82 +1255,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="13"/>
+      <c r="B2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="13"/>
+      <c r="B4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="B6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1345,20 +1346,167 @@
     <row r="11" spans="1:3" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="19"/>
+    </row>
+    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEFE42B-B445-084D-8420-40118E3748F8}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1381,12 +1529,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEFE42B-B445-084D-8420-40118E3748F8}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D64500-A598-ED4C-9FFB-4E8C0359C7ED}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1401,82 +1549,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1492,20 +1640,20 @@
     <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="21"/>
+      <c r="B12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1528,12 +1676,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D64500-A598-ED4C-9FFB-4E8C0359C7ED}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29C21F9-B739-8443-9C8D-FCC527CA221D}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1548,82 +1696,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="13"/>
+      <c r="B2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="B6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1639,184 +1787,37 @@
     <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="21"/>
+      <c r="B12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29C21F9-B739-8443-9C8D-FCC527CA221D}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="13"/>
-    </row>
-    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="13"/>
-    </row>
-    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="19"/>
-    </row>
-    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="21"/>
-    </row>
-    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1842,82 +1843,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="13"/>
+      <c r="B2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="19"/>
+      <c r="B3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="B6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="17"/>
+      <c r="B7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="17"/>
+      <c r="B8" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1933,37 +1934,37 @@
     <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="21"/>
+      <c r="B12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Class Diagram, added several features
</commit_message>
<xml_diff>
--- a/Use Case Descriptions.xlsx
+++ b/Use Case Descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niel/Documents/!TPADesktop/TPA-Desktop-LinKasa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E89130-EC08-4B41-A81D-DB9D425B873C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8170405F-0FFB-A345-8F06-D26187F8C0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="740" windowWidth="24720" windowHeight="16720" activeTab="5" xr2:uid="{B1ED97EC-A297-DE45-89E2-47350D4B0270}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="16720" xr2:uid="{B1ED97EC-A297-DE45-89E2-47350D4B0270}"/>
   </bookViews>
   <sheets>
     <sheet name="Update Lost and Found Entry" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Create Staff Data" sheetId="9" r:id="rId6"/>
     <sheet name="Public Chat Everyone" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,9 +108,6 @@
 Chief Operations Officer</t>
   </si>
   <si>
-    <t>Actor have to view real-time flight information first in order to manage certain flight schedule.</t>
-  </si>
-  <si>
     <t>Flight operations manager would like to create a new flight schedule.</t>
   </si>
   <si>
@@ -128,25 +125,6 @@
 3.2 System generates a success message.</t>
   </si>
   <si>
-    <t>1. Actor received a request to create a new flight schedule.
-2. Actor chooses to create a new flight.
-3. Actor inputs new flight schedule information.
-4. Actor receives a success message.</t>
-  </si>
-  <si>
-    <t>1.1 System creates a new form.
-1.2 System prompts staff to input item informations.
-2.1 System uploads a new data into database, which is the data for the newly found item.
-3.1 System updates the status according to staff's action.
-3.2 System displays a success message.</t>
-  </si>
-  <si>
-    <t>1. Lost and found staff would like to update the digital log with a newly found item.
-2. Lost and found staff inputs item name, description, and attaches image of the item.
-3. Lost and found staff sets the status either to "unclaimed" or "returned to owner".
-4. Lost and found staff receives a success message.</t>
-  </si>
-  <si>
     <t>Create a new flight schedule</t>
   </si>
   <si>
@@ -156,22 +134,13 @@
     <t>3.1 Some of the data are incomplete or flight number not unique for the following day.</t>
   </si>
   <si>
-    <t>Provide Baggage Information</t>
-  </si>
-  <si>
     <t>Flight operations manager create a new flight schedule to fulfill passenger's high demand on tickets.</t>
   </si>
   <si>
-    <t>Provide baggage information details</t>
-  </si>
-  <si>
     <t>Passengers check-in and drop their baggage before their flight.</t>
   </si>
   <si>
     <t>Check-in Staff</t>
-  </si>
-  <si>
-    <t>Check-in Staffs have to open the baggage handling information page in order to provide baggage information details.</t>
   </si>
   <si>
     <t>Passenger, Flight Crews</t>
@@ -189,12 +158,6 @@
 3.2 System generates success message.</t>
   </si>
   <si>
-    <t>1. Check-in Staff received a baggage to drop.
-2. Staff chooses to provide a new baggage information.
-3. Staff provides baggage detail information.
-4. Staff receives success message.</t>
-  </si>
-  <si>
     <t>3.1 Weight, dimension, or other detail informations incomplete.</t>
   </si>
   <si>
@@ -202,9 +165,6 @@
   </si>
   <si>
     <t>Assign flight crews into specific flight.</t>
-  </si>
-  <si>
-    <t>Flight Operations Manager could schedule several flight crews into specified flight especially for the newly added flight schedule.</t>
   </si>
   <si>
     <t>A new flight schedule that haven't had any flight crews.
@@ -217,10 +177,195 @@
     <t>Flight Attendants, Pilot</t>
   </si>
   <si>
-    <t>The selected flight schedule is updated with the newly assigned flight crews and uploaded to the database.</t>
-  </si>
-  <si>
-    <t>1.1 System shows list of flight crews page.
+    <t>1. Flight Operations Manager would like to assign flight crews to a specific flight schedule.
+2. Flight Operations Manager chooses the schedule from the list given.
+3. Flight Operations Manager chooses the crews for the specified flight schedule.
+4. Flight Operations Manager receives success message.</t>
+  </si>
+  <si>
+    <t>2.2 There are no available flight crews for the specified flight schedule.</t>
+  </si>
+  <si>
+    <t>Input Passenger Details</t>
+  </si>
+  <si>
+    <t>International passengers entering the international departures waiting room.</t>
+  </si>
+  <si>
+    <t>Customs and Border Control Officer</t>
+  </si>
+  <si>
+    <t>Input Passenger Personal Information, Passport, and Visa Details</t>
+  </si>
+  <si>
+    <t>Passenger information will be stored into database.
+Newly stored data will be updated along the system.</t>
+  </si>
+  <si>
+    <t>1.1 System creates a new form.
+1.2 System prompts officer to input passenger detail informations.
+2.1 System validates the inputted data.
+2.2 System uploads the inserted passenger information into the database.
+2.3 System displays success message.</t>
+  </si>
+  <si>
+    <t>1. Customs and Border Control Officer would like to input a new passenger detail.
+2. Customs and Border Control Officer inputs passenger's personal information, ID, passport, and visa details.
+3. Customs and Border Control Officer receives success message.</t>
+  </si>
+  <si>
+    <t>2.1 Passenger already exists in the passenger information or data incomplete.</t>
+  </si>
+  <si>
+    <t>Create Staff Data</t>
+  </si>
+  <si>
+    <t>Create new hired staff data.</t>
+  </si>
+  <si>
+    <t>Human Resources Director recently hired a new staff.</t>
+  </si>
+  <si>
+    <t>Human Resources Director</t>
+  </si>
+  <si>
+    <t>The data in "View detailed employee data" use case will be updated after executing the following use case.</t>
+  </si>
+  <si>
+    <t>New hired staff</t>
+  </si>
+  <si>
+    <t>A new staff data will be inserted into the database.
+Newly stored data will be updated along the system.</t>
+  </si>
+  <si>
+    <t>1. Human Resources Director hires a new staff.
+2. Human Resources Director input newly hired staff's data.
+3. Human Resources Director receives success message.</t>
+  </si>
+  <si>
+    <t>2.1 The inputted data was incomplete.
+2.2 Email generated must be unique.</t>
+  </si>
+  <si>
+    <t>Public Chat Everyone</t>
+  </si>
+  <si>
+    <t>Public Chat Everyone in the Airport.</t>
+  </si>
+  <si>
+    <t>An actor has an information to tell everyone at the airport.</t>
+  </si>
+  <si>
+    <t>Several actors at the airport could use the public chat feature to communicate with everyone at the airport.</t>
+  </si>
+  <si>
+    <t>Airport Operations Manager, Gate Agents, Ground Handling Manager, Landside Operations Manager, Customs and Border Control Officer, Baggage Security Supervisor, Cargo Handlers, Chief Operations Officer</t>
+  </si>
+  <si>
+    <t>The "Public Chat Everyone" use case itself would update its chat list whenever an actor sends a public chat.</t>
+  </si>
+  <si>
+    <t>Everyone at the airport.</t>
+  </si>
+  <si>
+    <t>The actor must be logged in and authorized to public chat.
+The chat database must be ready and available.</t>
+  </si>
+  <si>
+    <t>Human Resources Director must be logged in and authorized to create staff data.
+The new hired staff has the required information to create a new staff data.
+The staff database must be available and ready to use.</t>
+  </si>
+  <si>
+    <t>Customs and Border Control Officer must be logged in and authorized to input passenger details.
+Passenger details database must be available and ready to use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flight Operations Manager must be logged in and authorized to assign flight crews.
+The to be assigned flight schedule must exist in database.
+The specified flight crews must exist in database.
+</t>
+  </si>
+  <si>
+    <t>Check-in Staff must be logged in and authorized to provide baggage information.
+Baggage handling information page must be available.
+Baggage information such as dimensions, weight, and contents must be provided.</t>
+  </si>
+  <si>
+    <t>1.1 System opens chat room.
+1.2 System prompts actor to input public chat.
+2.1 System uploads sent chat to database.
+2.2 System updates the chat room.</t>
+  </si>
+  <si>
+    <t>The database will be updated according to the sent public chat.
+The public chat list will be updated in the system and for everyone at the airport.</t>
+  </si>
+  <si>
+    <t>1. Actor wants to send a public chat.
+2. Actor inputs chat and send the chat.
+3. Actor receives the newly sent chat message.</t>
+  </si>
+  <si>
+    <t>2.1 The inputted chat is empty.</t>
+  </si>
+  <si>
+    <t>Actor must be logged in and authorized to create flight schedule.
+Real-time flight schedule must exist.
+New flight schedule created must be unique.</t>
+  </si>
+  <si>
+    <t>View lost and found entry</t>
+  </si>
+  <si>
+    <t>Customer Service Manager, Information Desk Staff, Lost and Found Staff, Check-in Staff, Gate Agents, Airport Operations Manager, Flight Operations Manager, Ground Handling Manager, Landside Operations Manager, Maintenance Manager, Customs and Border Control Officers, Baggage Security Supervisor, Cargo Manager, Logistics Manager, Fuel Manager, Cargo Handlers, Civil Engineering Manager, Airport Director/CEO, Chief Financial Officer, Chief Operations Officer, Chief Security Officer, Human Resources Director</t>
+  </si>
+  <si>
+    <t>Lost and found staff must be logged in and authorized to update lost and found entry.
+Lost and found log must exists.
+The digital log must be created.
+A lost item has been reported.</t>
+  </si>
+  <si>
+    <t>2.1 Some of the data is incomplete or status is not selected</t>
+  </si>
+  <si>
+    <t>View flight crews, Access passenger information</t>
+  </si>
+  <si>
+    <t>Access Passenger Information</t>
+  </si>
+  <si>
+    <t>Passenger, Check-in Staff, Customs and Border Control Officers, Flight Operations Manager, Gate Agents</t>
+  </si>
+  <si>
+    <t>Customs and Border Control Officer could manually input the passenger's personal information such as Full Name, Date of Birth, Nationality, Passport Number, and Visa details before entering the departures waiting room.</t>
+  </si>
+  <si>
+    <t>Human Resources Director could insert new staff data such as name, role, address, date of birth into database, then generate email and password for recently hired staff.</t>
+  </si>
+  <si>
+    <t>1.1 System creates a new form.
+1.2 System prompts staff to input item informations, such as name, description, and attach an image of the item.
+2.1 System uploads a new data into database, which is the data for the newly found item.
+3.1 System updates the status according to staff's action.
+3.2 System displays a success message.</t>
+  </si>
+  <si>
+    <t>1. Lost and found staff would like to update the digital log with a recently found item.
+2. Lost and found staff inputs item name, description, and attaches image of the item.
+3. Lost and found staff sets the status either to "unclaimed" or "returned to owner".
+4. Lost and found staff receives a success message.</t>
+  </si>
+  <si>
+    <t>Flight Operations Manager could schedule several flight crews into specified flight especially for the recently added flight schedule.</t>
+  </si>
+  <si>
+    <t>The selected flight schedule is updated with the recently assigned flight crews and uploaded to the database.</t>
+  </si>
+  <si>
+    <t>1.1 System shows list of flight schedules.
 1.2 System prompts manager to select the specified flight schedule
 2.1 System shows the flight crews that are available for the following flight schedule.
 2.2 System prompts user to select the flight crews.
@@ -228,183 +373,39 @@
 3.2 System displays success message.</t>
   </si>
   <si>
-    <t>1. Flight Operations Manager would like to assign flight crews to a specific flight schedule.
-2. Flight Operations Manager chooses the schedule from the list given.
-3. Flight Operations Manager chooses the crews for the specified flight schedule.
-4. Flight Operations Manager receives success message.</t>
-  </si>
-  <si>
-    <t>2.2 There are no available flight crews for the specified flight schedule.</t>
-  </si>
-  <si>
-    <t>Input Passenger Details</t>
-  </si>
-  <si>
-    <t>International passengers entering the international departures waiting room.</t>
-  </si>
-  <si>
-    <t>Customs and Border Control Officer</t>
-  </si>
-  <si>
-    <t>Input Passenger Personal Information, Passport, and Visa Details</t>
-  </si>
-  <si>
-    <t>Passenger information will be stored into database.
-Newly stored data will be updated along the system.</t>
-  </si>
-  <si>
-    <t>1.1 System creates a new form.
-1.2 System prompts officer to input passenger detail informations.
-2.1 System validates the inputted data.
-2.2 System uploads the inserted passenger information into the database.
-2.3 System displays success message.</t>
-  </si>
-  <si>
-    <t>1. Customs and Border Control Officer would like to input a new passenger detail.
-2. Customs and Border Control Officer inputs passenger's personal information, ID, passport, and visa details.
-3. Customs and Border Control Officer receives success message.</t>
-  </si>
-  <si>
-    <t>2.1 Passenger already exists in the passenger information or data incomplete.</t>
-  </si>
-  <si>
-    <t>Create Staff Data</t>
-  </si>
-  <si>
-    <t>Create new hired staff data.</t>
-  </si>
-  <si>
-    <t>Human Resources Director recently hired a new staff.</t>
-  </si>
-  <si>
-    <t>Human Resources Director</t>
-  </si>
-  <si>
-    <t>The data in "View detailed employee data" use case will be updated after executing the following use case.</t>
-  </si>
-  <si>
-    <t>New hired staff</t>
-  </si>
-  <si>
-    <t>A new staff data will be inserted into the database.
-Newly stored data will be updated along the system.</t>
+    <t>View real-time flight information</t>
+  </si>
+  <si>
+    <t>Add baggage details</t>
+  </si>
+  <si>
+    <t>Provide baggage information and details</t>
+  </si>
+  <si>
+    <t>View baggage handling information</t>
+  </si>
+  <si>
+    <t>1. Actor received a request to create a new flight schedule.
+2. Actor chooses to create a new flight.
+3. Actor inputs new flight schedule information, such as flight number, flight schedule, flight origin, and flight destination.
+4. Actor receives a success message.</t>
   </si>
   <si>
     <t>1.1 System creates a new form.
 1.2 System prompts director to input staff data.
 2.1 System validates the inputted data.
-2.2 System generates the email based on the specified format.
+2.2 System generates the email based on the specified format, such as [first name].[last name]@linkasa.co.
+2.3 System generates the password based on the specified format, such as linkasa[dob in yyyy-MM-dd format].
 2.3 System displays success message.</t>
   </si>
   <si>
-    <t>1. Human Resources Director hires a new staff.
-2. Human Resources Director input newly hired staff's data.
-3. Human Resources Director receives success message.</t>
-  </si>
-  <si>
-    <t>2.1 The inputted data was incomplete.
-2.2 Email generated must be unique.</t>
-  </si>
-  <si>
-    <t>Public Chat Everyone</t>
-  </si>
-  <si>
-    <t>Public Chat Everyone in the Airport.</t>
-  </si>
-  <si>
-    <t>An actor has an information to tell everyone at the airport.</t>
-  </si>
-  <si>
-    <t>Several actors at the airport could use the public chat feature to communicate with everyone at the airport.</t>
-  </si>
-  <si>
-    <t>Airport Operations Manager, Gate Agents, Ground Handling Manager, Landside Operations Manager, Customs and Border Control Officer, Baggage Security Supervisor, Cargo Handlers, Chief Operations Officer</t>
-  </si>
-  <si>
-    <t>The "Public Chat Everyone" use case itself would update its chat list whenever an actor sends a public chat.</t>
-  </si>
-  <si>
-    <t>Everyone at the airport.</t>
-  </si>
-  <si>
-    <t>The actor must be logged in and authorized to public chat.
-The chat database must be ready and available.</t>
-  </si>
-  <si>
-    <t>Human Resources Director must be logged in and authorized to create staff data.
-The new hired staff has the required information to create a new staff data.
-The staff database must be available and ready to use.</t>
-  </si>
-  <si>
-    <t>Customs and Border Control Officer must be logged in and authorized to input passenger details.
-Passenger details database must be available and ready to use.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flight Operations Manager must be logged in and authorized to assign flight crews.
-The to be assigned flight schedule must exist in database.
-The specified flight crews must exist in database.
-</t>
-  </si>
-  <si>
-    <t>Check-in Staff must be logged in and authorized to provide baggage information.
-Baggage handling information page must be available.
-Baggage information such as dimensions, weight, and contents must be provided.</t>
-  </si>
-  <si>
-    <t>1.1 System opens chat room.
-1.2 System prompts actor to input public chat.
-2.1 System uploads sent chat to database.
-2.2 System updates the chat room.</t>
-  </si>
-  <si>
-    <t>The database will be updated according to the sent public chat.
-The public chat list will be updated in the system and for everyone at the airport.</t>
-  </si>
-  <si>
-    <t>1. Actor wants to send a public chat.
-2. Actor inputs chat and send the chat.
-3. Actor receives the newly sent chat message.</t>
-  </si>
-  <si>
-    <t>2.1 The inputted chat is empty.</t>
-  </si>
-  <si>
-    <t>Actor must be logged in and authorized to create flight schedule.
-Real-time flight schedule must exist.
-New flight schedule created must be unique.</t>
-  </si>
-  <si>
-    <t>View lost and found entry</t>
-  </si>
-  <si>
-    <t>Customer Service Manager, Information Desk Staff, Lost and Found Staff, Check-in Staff, Gate Agents, Airport Operations Manager, Flight Operations Manager, Ground Handling Manager, Landside Operations Manager, Maintenance Manager, Customs and Border Control Officers, Baggage Security Supervisor, Cargo Manager, Logistics Manager, Fuel Manager, Cargo Handlers, Civil Engineering Manager, Airport Director/CEO, Chief Financial Officer, Chief Operations Officer, Chief Security Officer, Human Resources Director</t>
-  </si>
-  <si>
-    <t>Lost and found staff must be logged in and authorized to update lost and found entry.
-Lost and found log must exists.
-The digital log must be created.
-A lost item has been reported.</t>
-  </si>
-  <si>
-    <t>2.1 Some of the data is incomplete or status is not selected</t>
-  </si>
-  <si>
-    <t>Provide detailed baggage information such as weight, dimensions, content, and attach photos.</t>
-  </si>
-  <si>
-    <t>View flight crews, Access passenger information</t>
-  </si>
-  <si>
-    <t>Access Passenger Information</t>
-  </si>
-  <si>
-    <t>Passenger, Check-in Staff, Customs and Border Control Officers, Flight Operations Manager, Gate Agents</t>
-  </si>
-  <si>
-    <t>Customs and Border Control Officer could manually input the passenger's personal information such as Full Name, Date of Birth, Nationality, Passport Number, and Visa details before entering the departures waiting room.</t>
-  </si>
-  <si>
-    <t>Human Resources Director could insert new staff data such as name, role, address, date of birth into database, then generate email and password for recently hired staff.</t>
+    <t>1. Check-in Staff received a baggage to drop.
+2. Staff chooses to provide a new baggage information, such as weight, dimensions and attach photos.
+3. Staff provides baggage detail information.
+4. Staff receives success message.</t>
+  </si>
+  <si>
+    <t>Provide detailed baggage information such as weight, dimensions, and attach photos.</t>
   </si>
 </sst>
 </file>
@@ -593,6 +594,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -608,26 +612,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -945,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABC9673-1384-A541-9754-03D8B487CAC3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -961,82 +962,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="21"/>
+      <c r="B7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="B8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1052,20 +1053,20 @@
     <row r="11" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1092,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F06FCE-2A99-3641-B0B3-A6FEC9347627}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1108,82 +1109,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="14"/>
+      <c r="B6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="15"/>
+      <c r="B7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="B8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1199,37 +1200,37 @@
     <row r="11" spans="1:3" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="19"/>
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1240,7 +1241,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1255,82 +1256,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="17"/>
+      <c r="B3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="14"/>
+      <c r="B6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="15"/>
+      <c r="B7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="B8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1346,20 +1347,167 @@
     <row r="11" spans="1:3" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="19"/>
+      <c r="B12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEFE42B-B445-084D-8420-40118E3748F8}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1382,12 +1530,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEFE42B-B445-084D-8420-40118E3748F8}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D64500-A598-ED4C-9FFB-4E8C0359C7ED}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1402,82 +1550,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="12"/>
+      <c r="B5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="B8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1490,23 +1638,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="192" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="19"/>
+      <c r="B12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1529,12 +1677,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D64500-A598-ED4C-9FFB-4E8C0359C7ED}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29C21F9-B739-8443-9C8D-FCC527CA221D}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1549,82 +1697,82 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="14"/>
+      <c r="B4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="15"/>
+      <c r="B7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="B8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1637,23 +1785,170 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="231" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720AF24D-E198-FC42-906F-2832386300DE}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="112" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>58</v>
       </c>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="19"/>
+    </row>
+    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="19"/>
+      <c r="B12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -1674,298 +1969,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29C21F9-B739-8443-9C8D-FCC527CA221D}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720AF24D-E198-FC42-906F-2832386300DE}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView zoomScale="112" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="240" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>